<commit_message>
fix dBFS integer input bug, disable window resize, disable inputs while convert
</commit_message>
<xml_diff>
--- a/update list.xlsx
+++ b/update list.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>bugs /to be revised</t>
   </si>
@@ -31,28 +31,25 @@
     <t>v</t>
   </si>
   <si>
-    <t>cmd window不該出現</t>
-  </si>
-  <si>
     <t>normalize不能輸入小數，沒做正負特判</t>
   </si>
   <si>
-    <t>revise .mp4 to .m4a(AAC or ALAC), support  FLAC(.flac)</t>
-  </si>
-  <si>
-    <t>在加入queue前可選擇下載影片或音檔</t>
-  </si>
-  <si>
-    <t>更改console成多個blocks，可刪除或修改block</t>
-  </si>
-  <si>
-    <t>use listbox</t>
-  </si>
-  <si>
-    <t>ping 的取代方案</t>
-  </si>
-  <si>
-    <t>pytube再次出問題，目前等待修復中</t>
+    <t>support  AAC(.m4a), FLAC(.flac), WMA(.wma), WAV(wav), MP3(.mp3)</t>
+  </si>
+  <si>
+    <t>需要在convert時鎖定所有輸入</t>
+  </si>
+  <si>
+    <t>禁止螢幕縮放</t>
+  </si>
+  <si>
+    <t>允許使用playlist url下載整個playlist內的音檔</t>
+  </si>
+  <si>
+    <t>執行效能顯然有待加強，集中管理未完成的urls、Youtube objects，只取得Youtube objects一次</t>
+  </si>
+  <si>
+    <t>urls已完成</t>
   </si>
 </sst>
 </file>
@@ -120,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,12 +129,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -448,15 +439,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="78.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="105.57642857142856" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="6.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -484,53 +475,50 @@
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="21">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="C4" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="22.5">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="3" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3"/>
       <c r="C8" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="22.5">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>